<commit_message>
Rebuilt the df module.
</commit_message>
<xml_diff>
--- a/data/excel/sample.xlsx
+++ b/data/excel/sample.xlsx
@@ -1,34 +1,68 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hayma\PycharmProjects\poap\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892D8491-4CBC-4E3A-A1D5-5BC8F8B43F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F4BCA5-D0F1-4834-8B99-AE5B8E57BA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="settings" sheetId="1" r:id="rId1"/>
+    <sheet name="tasks" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>help</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>The height of the object</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>The width of the object</t>
+  </si>
+  <si>
+    <t>rows</t>
+  </si>
+  <si>
+    <t>The number of rows in the object</t>
+  </si>
+  <si>
+    <t>task</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>finish</t>
+  </si>
+  <si>
+    <t>task1</t>
+  </si>
+  <si>
+    <t>task2</t>
+  </si>
+  <si>
+    <t>task3</t>
   </si>
 </sst>
 </file>
@@ -84,11 +118,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,54 +428,120 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>200</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2">
+        <v>45366</v>
+      </c>
+      <c r="D2" s="2">
+        <v>45371</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2">
+        <v>45376</v>
+      </c>
+      <c r="D3" s="2">
+        <v>45381</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2">
+        <v>45392</v>
+      </c>
+      <c r="D4" s="2">
+        <v>45402</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved gui.py and added logo
</commit_message>
<xml_diff>
--- a/data/excel/sample.xlsx
+++ b/data/excel/sample.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,77 +450,107 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>start</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2024-01-01</t>
-        </is>
+          <t>page_width</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>200</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>The start date of the project</t>
+          <t>The width of the page in arbitrary units</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>resolution</t>
+          <t>page_height</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Pixels per day</t>
+          <t>The height of the page in arbitrary units</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>width</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>200</v>
+          <t>start_date</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2024-01-01</t>
+        </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>The height of the object</t>
+          <t>The start date of the chart</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>height</t>
+          <t>header_height</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>100</v>
+        <v>0.1</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>The width of the object</t>
+          <t>The height of the header as a proportion of the page height</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>rows</t>
+          <t>footer_height</t>
         </is>
       </c>
       <c r="B6" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>The height of the footer as a proportion of the page height</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>total_scale_height</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>The total height available for scales as a proportion of the page height</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>row_quantity</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>5</v>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>The number of rows in the object</t>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>The number of rows in the chart</t>
         </is>
       </c>
     </row>

</xml_diff>